<commit_message>
- update requirements file - update README - update cpi data file - update example notebook for Sep
</commit_message>
<xml_diff>
--- a/data/statssa_cpi.xlsx
+++ b/data/statssa_cpi.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andrew\SAS tutorials\Prog3\Prices Manuals\CPI\CPI release and CD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DATA\econstats\Prices\P0141_CPI\P0141_CPI\Releases\Release\RELEASES2023\August 2023\Timeseries\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2401" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2404" uniqueCount="633">
   <si>
     <t>H01</t>
   </si>
@@ -1918,6 +1918,9 @@
   </si>
   <si>
     <t>M202307</t>
+  </si>
+  <si>
+    <t>M202308</t>
   </si>
 </sst>
 </file>
@@ -1927,7 +1930,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -2257,24 +2260,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CI229"/>
+  <dimension ref="A1:CJ229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BG1" workbookViewId="0">
-      <selection activeCell="CI1" sqref="CI1"/>
+    <sheetView tabSelected="1" topLeftCell="BT1" workbookViewId="0">
+      <selection activeCell="CJ227" sqref="CJ2:CJ227"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
-    <col min="5" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" style="2" customWidth="1"/>
-    <col min="9" max="66" width="8.85546875" customWidth="1"/>
-    <col min="69" max="69" width="8.85546875" style="1"/>
-    <col min="79" max="79" width="8.85546875" style="1"/>
-    <col min="81" max="81" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="5" max="7" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="2" customWidth="1"/>
+    <col min="9" max="66" width="8.88671875" customWidth="1"/>
+    <col min="69" max="69" width="8.88671875" style="1"/>
+    <col min="79" max="79" width="8.88671875" style="1"/>
+    <col min="81" max="81" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:88">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2536,8 +2539,11 @@
       <c r="CI1" s="3" t="s">
         <v>631</v>
       </c>
+      <c r="CJ1" s="3" t="s">
+        <v>632</v>
+      </c>
     </row>
-    <row r="2" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:88">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -2799,8 +2805,11 @@
       <c r="CI2" s="1">
         <v>118.8</v>
       </c>
+      <c r="CJ2" s="1">
+        <v>122.8</v>
+      </c>
     </row>
-    <row r="3" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:88">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -3062,8 +3071,11 @@
       <c r="CI3" s="1">
         <v>119.4</v>
       </c>
+      <c r="CJ3" s="1">
+        <v>119.3</v>
+      </c>
     </row>
-    <row r="4" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:88">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3325,8 +3337,11 @@
       <c r="CI4" s="1">
         <v>123</v>
       </c>
+      <c r="CJ4" s="1">
+        <v>122.3</v>
+      </c>
     </row>
-    <row r="5" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:88">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -3588,8 +3603,11 @@
       <c r="CI5" s="1">
         <v>126.1</v>
       </c>
+      <c r="CJ5" s="1">
+        <v>127.1</v>
+      </c>
     </row>
-    <row r="6" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:88">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -3851,8 +3869,11 @@
       <c r="CI6" s="1">
         <v>123.2</v>
       </c>
+      <c r="CJ6" s="1">
+        <v>123.3</v>
+      </c>
     </row>
-    <row r="7" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:88">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -4114,8 +4135,11 @@
       <c r="CI7" s="1">
         <v>121.3</v>
       </c>
+      <c r="CJ7" s="1">
+        <v>122.1</v>
+      </c>
     </row>
-    <row r="8" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:88">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -4377,8 +4401,11 @@
       <c r="CI8" s="1">
         <v>115.7</v>
       </c>
+      <c r="CJ8" s="1">
+        <v>115.6</v>
+      </c>
     </row>
-    <row r="9" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:88">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -4640,8 +4667,11 @@
       <c r="CI9" s="1">
         <v>123</v>
       </c>
+      <c r="CJ9" s="1">
+        <v>124.2</v>
+      </c>
     </row>
-    <row r="10" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:88">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -4903,8 +4933,11 @@
       <c r="CI10" s="1">
         <v>126.7</v>
       </c>
+      <c r="CJ10" s="1">
+        <v>127.6</v>
+      </c>
     </row>
-    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:88">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -5166,8 +5199,11 @@
       <c r="CI11" s="1">
         <v>123.2</v>
       </c>
+      <c r="CJ11" s="1">
+        <v>123.2</v>
+      </c>
     </row>
-    <row r="12" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:88">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -5429,8 +5465,11 @@
       <c r="CI12" s="1">
         <v>136.5</v>
       </c>
+      <c r="CJ12" s="1">
+        <v>136.6</v>
+      </c>
     </row>
-    <row r="13" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:88">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -5692,8 +5731,11 @@
       <c r="CI13" s="1">
         <v>116.6</v>
       </c>
+      <c r="CJ13" s="1">
+        <v>116.9</v>
+      </c>
     </row>
-    <row r="14" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:88">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -5955,8 +5997,11 @@
       <c r="CI14" s="1">
         <v>132.4</v>
       </c>
+      <c r="CJ14" s="1">
+        <v>134.80000000000001</v>
+      </c>
     </row>
-    <row r="15" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:88">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -6218,8 +6263,11 @@
       <c r="CI15" s="1">
         <v>138.30000000000001</v>
       </c>
+      <c r="CJ15" s="1">
+        <v>138.6</v>
+      </c>
     </row>
-    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:88">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -6481,8 +6529,11 @@
       <c r="CI16" s="1">
         <v>127.9</v>
       </c>
+      <c r="CJ16" s="1">
+        <v>127.9</v>
+      </c>
     </row>
-    <row r="17" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:88">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -6744,8 +6795,11 @@
       <c r="CI17" s="1">
         <v>142.1</v>
       </c>
+      <c r="CJ17" s="1">
+        <v>140.80000000000001</v>
+      </c>
     </row>
-    <row r="18" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:88">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -7007,8 +7061,11 @@
       <c r="CI18" s="1">
         <v>128.19999999999999</v>
       </c>
+      <c r="CJ18" s="1">
+        <v>127.8</v>
+      </c>
     </row>
-    <row r="19" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:88">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -7270,8 +7327,11 @@
       <c r="CI19" s="7" t="s">
         <v>523</v>
       </c>
+      <c r="CJ19" s="7" t="s">
+        <v>523</v>
+      </c>
     </row>
-    <row r="20" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:88">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -7533,8 +7593,11 @@
       <c r="CI20" s="7" t="s">
         <v>523</v>
       </c>
+      <c r="CJ20" s="7" t="s">
+        <v>523</v>
+      </c>
     </row>
-    <row r="21" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:88">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -7796,8 +7859,11 @@
       <c r="CI21" s="1">
         <v>124.9</v>
       </c>
+      <c r="CJ21" s="1">
+        <v>119.5</v>
+      </c>
     </row>
-    <row r="22" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:88">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -8059,8 +8125,11 @@
       <c r="CI22" s="1">
         <v>114.4</v>
       </c>
+      <c r="CJ22" s="1">
+        <v>114.7</v>
+      </c>
     </row>
-    <row r="23" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:88">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -8322,8 +8391,11 @@
       <c r="CI23" s="1">
         <v>138.4</v>
       </c>
+      <c r="CJ23" s="1">
+        <v>137.80000000000001</v>
+      </c>
     </row>
-    <row r="24" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:88">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -8585,8 +8657,11 @@
       <c r="CI24" s="1">
         <v>108.5</v>
       </c>
+      <c r="CJ24" s="1">
+        <v>107.5</v>
+      </c>
     </row>
-    <row r="25" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:88">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -8848,8 +8923,11 @@
       <c r="CI25" s="1">
         <v>112.6</v>
       </c>
+      <c r="CJ25" s="1">
+        <v>109.8</v>
+      </c>
     </row>
-    <row r="26" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:88">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -9111,8 +9189,11 @@
       <c r="CI26" s="1">
         <v>113.9</v>
       </c>
+      <c r="CJ26" s="1">
+        <v>111.8</v>
+      </c>
     </row>
-    <row r="27" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:88">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -9374,8 +9455,11 @@
       <c r="CI27" s="1">
         <v>105.3</v>
       </c>
+      <c r="CJ27" s="1">
+        <v>105</v>
+      </c>
     </row>
-    <row r="28" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:88">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -9637,8 +9721,11 @@
       <c r="CI28" s="1">
         <v>105.9</v>
       </c>
+      <c r="CJ28" s="1">
+        <v>107.1</v>
+      </c>
     </row>
-    <row r="29" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:88">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -9900,8 +9987,11 @@
       <c r="CI29" s="1">
         <v>105.9</v>
       </c>
+      <c r="CJ29" s="1">
+        <v>106.1</v>
+      </c>
     </row>
-    <row r="30" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:88">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -10163,8 +10253,11 @@
       <c r="CI30" s="1">
         <v>113.7</v>
       </c>
+      <c r="CJ30" s="1">
+        <v>110.1</v>
+      </c>
     </row>
-    <row r="31" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:88">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -10426,8 +10519,11 @@
       <c r="CI31" s="1">
         <v>117.2</v>
       </c>
+      <c r="CJ31" s="1">
+        <v>114.6</v>
+      </c>
     </row>
-    <row r="32" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:88">
       <c r="A32" t="s">
         <v>39</v>
       </c>
@@ -10689,8 +10785,11 @@
       <c r="CI32" s="1">
         <v>115.4</v>
       </c>
+      <c r="CJ32" s="1">
+        <v>114.9</v>
+      </c>
     </row>
-    <row r="33" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:88">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -10952,8 +11051,11 @@
       <c r="CI33" s="1">
         <v>115.9</v>
       </c>
+      <c r="CJ33" s="1">
+        <v>114</v>
+      </c>
     </row>
-    <row r="34" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:88">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -11215,8 +11317,11 @@
       <c r="CI34" s="1">
         <v>114.2</v>
       </c>
+      <c r="CJ34" s="1">
+        <v>114.3</v>
+      </c>
     </row>
-    <row r="35" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:88">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -11478,8 +11583,11 @@
       <c r="CI35" s="1">
         <v>112.1</v>
       </c>
+      <c r="CJ35" s="1">
+        <v>111.2</v>
+      </c>
     </row>
-    <row r="36" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:88">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -11741,8 +11849,11 @@
       <c r="CI36" s="1">
         <v>114.8</v>
       </c>
+      <c r="CJ36" s="1">
+        <v>117.4</v>
+      </c>
     </row>
-    <row r="37" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:88">
       <c r="A37" t="s">
         <v>39</v>
       </c>
@@ -12004,8 +12115,11 @@
       <c r="CI37" s="1">
         <v>108.3</v>
       </c>
+      <c r="CJ37" s="1">
+        <v>109.3</v>
+      </c>
     </row>
-    <row r="38" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:88">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -12267,8 +12381,11 @@
       <c r="CI38" s="1">
         <v>125.1</v>
       </c>
+      <c r="CJ38" s="1">
+        <v>124.9</v>
+      </c>
     </row>
-    <row r="39" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:88">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -12530,8 +12647,11 @@
       <c r="CI39" s="1">
         <v>111.1</v>
       </c>
+      <c r="CJ39" s="1">
+        <v>111</v>
+      </c>
     </row>
-    <row r="40" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:88">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -12793,8 +12913,11 @@
       <c r="CI40" s="1">
         <v>115.9</v>
       </c>
+      <c r="CJ40" s="1">
+        <v>117</v>
+      </c>
     </row>
-    <row r="41" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:88">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -13056,8 +13179,11 @@
       <c r="CI41" s="1">
         <v>125.2</v>
       </c>
+      <c r="CJ41" s="1">
+        <v>125.1</v>
+      </c>
     </row>
-    <row r="42" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:88">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -13319,8 +13445,11 @@
       <c r="CI42" s="1">
         <v>112.5</v>
       </c>
+      <c r="CJ42" s="1">
+        <v>111.6</v>
+      </c>
     </row>
-    <row r="43" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:88">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -13582,8 +13711,11 @@
       <c r="CI43" s="1">
         <v>117.8</v>
       </c>
+      <c r="CJ43" s="1">
+        <v>120.4</v>
+      </c>
     </row>
-    <row r="44" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:88">
       <c r="A44" t="s">
         <v>39</v>
       </c>
@@ -13845,8 +13977,11 @@
       <c r="CI44" s="1">
         <v>113.6</v>
       </c>
+      <c r="CJ44" s="1">
+        <v>116.5</v>
+      </c>
     </row>
-    <row r="45" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:88">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -14108,8 +14243,11 @@
       <c r="CI45" s="1">
         <v>120</v>
       </c>
+      <c r="CJ45" s="1">
+        <v>119.7</v>
+      </c>
     </row>
-    <row r="46" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:88">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -14371,8 +14509,11 @@
       <c r="CI46" s="1">
         <v>123.6</v>
       </c>
+      <c r="CJ46" s="1">
+        <v>123.2</v>
+      </c>
     </row>
-    <row r="47" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:88">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -14634,8 +14775,11 @@
       <c r="CI47" s="1">
         <v>122.4</v>
       </c>
+      <c r="CJ47" s="1">
+        <v>123.2</v>
+      </c>
     </row>
-    <row r="48" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:88">
       <c r="A48" t="s">
         <v>39</v>
       </c>
@@ -14897,8 +15041,11 @@
       <c r="CI48" s="1">
         <v>121.6</v>
       </c>
+      <c r="CJ48" s="1">
+        <v>120.6</v>
+      </c>
     </row>
-    <row r="49" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:88">
       <c r="A49" t="s">
         <v>39</v>
       </c>
@@ -15160,8 +15307,11 @@
       <c r="CI49" s="1">
         <v>114.1</v>
       </c>
+      <c r="CJ49" s="1">
+        <v>115.3</v>
+      </c>
     </row>
-    <row r="50" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:88">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -15423,8 +15573,11 @@
       <c r="CI50" s="1">
         <v>116.5</v>
       </c>
+      <c r="CJ50" s="1">
+        <v>117.1</v>
+      </c>
     </row>
-    <row r="51" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:88">
       <c r="A51" t="s">
         <v>39</v>
       </c>
@@ -15686,8 +15839,11 @@
       <c r="CI51" s="1">
         <v>124.6</v>
       </c>
+      <c r="CJ51" s="1">
+        <v>126.7</v>
+      </c>
     </row>
-    <row r="52" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:88">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -15949,8 +16105,11 @@
       <c r="CI52" s="1">
         <v>120.9</v>
       </c>
+      <c r="CJ52" s="1">
+        <v>123.1</v>
+      </c>
     </row>
-    <row r="53" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:88">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -16212,8 +16371,11 @@
       <c r="CI53" s="1">
         <v>119.4</v>
       </c>
+      <c r="CJ53" s="1">
+        <v>119.2</v>
+      </c>
     </row>
-    <row r="54" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:88">
       <c r="A54" t="s">
         <v>39</v>
       </c>
@@ -16475,8 +16637,11 @@
       <c r="CI54" s="1">
         <v>115.2</v>
       </c>
+      <c r="CJ54" s="1">
+        <v>113.4</v>
+      </c>
     </row>
-    <row r="55" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:88">
       <c r="A55" t="s">
         <v>39</v>
       </c>
@@ -16738,8 +16903,11 @@
       <c r="CI55" s="1">
         <v>122.6</v>
       </c>
+      <c r="CJ55" s="1">
+        <v>121</v>
+      </c>
     </row>
-    <row r="56" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:88">
       <c r="A56" t="s">
         <v>39</v>
       </c>
@@ -17001,8 +17169,11 @@
       <c r="CI56" s="1">
         <v>120.8</v>
       </c>
+      <c r="CJ56" s="1">
+        <v>120.2</v>
+      </c>
     </row>
-    <row r="57" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:88">
       <c r="A57" t="s">
         <v>39</v>
       </c>
@@ -17264,8 +17435,11 @@
       <c r="CI57" s="1">
         <v>126.9</v>
       </c>
+      <c r="CJ57" s="1">
+        <v>128</v>
+      </c>
     </row>
-    <row r="58" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:88">
       <c r="A58" t="s">
         <v>39</v>
       </c>
@@ -17527,8 +17701,11 @@
       <c r="CI58" s="1">
         <v>115.1</v>
       </c>
+      <c r="CJ58" s="1">
+        <v>116.6</v>
+      </c>
     </row>
-    <row r="59" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:88">
       <c r="A59" t="s">
         <v>39</v>
       </c>
@@ -17790,8 +17967,11 @@
       <c r="CI59" s="1">
         <v>112.1</v>
       </c>
+      <c r="CJ59" s="1">
+        <v>111.8</v>
+      </c>
     </row>
-    <row r="60" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:88">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -18053,8 +18233,11 @@
       <c r="CI60" s="1">
         <v>121</v>
       </c>
+      <c r="CJ60" s="1">
+        <v>121.8</v>
+      </c>
     </row>
-    <row r="61" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:88">
       <c r="A61" t="s">
         <v>39</v>
       </c>
@@ -18316,8 +18499,11 @@
       <c r="CI61" s="1">
         <v>116.7</v>
       </c>
+      <c r="CJ61" s="1">
+        <v>117.6</v>
+      </c>
     </row>
-    <row r="62" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:88">
       <c r="A62" t="s">
         <v>39</v>
       </c>
@@ -18579,8 +18765,11 @@
       <c r="CI62" s="1">
         <v>115.7</v>
       </c>
+      <c r="CJ62" s="1">
+        <v>115.1</v>
+      </c>
     </row>
-    <row r="63" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:88">
       <c r="A63" t="s">
         <v>39</v>
       </c>
@@ -18842,8 +19031,11 @@
       <c r="CI63" s="1">
         <v>117.2</v>
       </c>
+      <c r="CJ63" s="1">
+        <v>117.2</v>
+      </c>
     </row>
-    <row r="64" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:88">
       <c r="A64" t="s">
         <v>39</v>
       </c>
@@ -19105,8 +19297,11 @@
       <c r="CI64" s="1">
         <v>120.6</v>
       </c>
+      <c r="CJ64" s="1">
+        <v>120.1</v>
+      </c>
     </row>
-    <row r="65" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:88">
       <c r="A65" t="s">
         <v>39</v>
       </c>
@@ -19368,8 +19563,11 @@
       <c r="CI65" s="1">
         <v>118.8</v>
       </c>
+      <c r="CJ65" s="1">
+        <v>118.6</v>
+      </c>
     </row>
-    <row r="66" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:88">
       <c r="A66" t="s">
         <v>39</v>
       </c>
@@ -19631,8 +19829,11 @@
       <c r="CI66" s="1">
         <v>113.3</v>
       </c>
+      <c r="CJ66" s="1">
+        <v>113.2</v>
+      </c>
     </row>
-    <row r="67" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:88">
       <c r="A67" t="s">
         <v>39</v>
       </c>
@@ -19894,8 +20095,11 @@
       <c r="CI67" s="1">
         <v>104.9</v>
       </c>
+      <c r="CJ67" s="1">
+        <v>106.9</v>
+      </c>
     </row>
-    <row r="68" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:88">
       <c r="A68" t="s">
         <v>39</v>
       </c>
@@ -20157,8 +20361,11 @@
       <c r="CI68" s="1">
         <v>115.8</v>
       </c>
+      <c r="CJ68" s="1">
+        <v>115.8</v>
+      </c>
     </row>
-    <row r="69" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:88">
       <c r="A69" t="s">
         <v>39</v>
       </c>
@@ -20420,8 +20627,11 @@
       <c r="CI69" s="1">
         <v>100.5</v>
       </c>
+      <c r="CJ69" s="1">
+        <v>103.1</v>
+      </c>
     </row>
-    <row r="70" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:88">
       <c r="A70" t="s">
         <v>39</v>
       </c>
@@ -20683,8 +20893,11 @@
       <c r="CI70" s="1">
         <v>111</v>
       </c>
+      <c r="CJ70" s="1">
+        <v>112.1</v>
+      </c>
     </row>
-    <row r="71" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:88">
       <c r="A71" t="s">
         <v>39</v>
       </c>
@@ -20946,8 +21159,11 @@
       <c r="CI71" s="1">
         <v>82.3</v>
       </c>
+      <c r="CJ71" s="1">
+        <v>83.3</v>
+      </c>
     </row>
-    <row r="72" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:88">
       <c r="A72" t="s">
         <v>39</v>
       </c>
@@ -21209,8 +21425,11 @@
       <c r="CI72" s="1">
         <v>104.9</v>
       </c>
+      <c r="CJ72" s="1">
+        <v>106.1</v>
+      </c>
     </row>
-    <row r="73" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:88">
       <c r="A73" t="s">
         <v>39</v>
       </c>
@@ -21472,8 +21691,11 @@
       <c r="CI73" s="1">
         <v>117.1</v>
       </c>
+      <c r="CJ73" s="1">
+        <v>124</v>
+      </c>
     </row>
-    <row r="74" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:88">
       <c r="A74" t="s">
         <v>39</v>
       </c>
@@ -21735,8 +21957,11 @@
       <c r="CI74" s="1">
         <v>127.5</v>
       </c>
+      <c r="CJ74" s="1">
+        <v>131.1</v>
+      </c>
     </row>
-    <row r="75" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:88">
       <c r="A75" t="s">
         <v>39</v>
       </c>
@@ -21998,8 +22223,11 @@
       <c r="CI75" s="1">
         <v>126.7</v>
       </c>
+      <c r="CJ75" s="1">
+        <v>125.8</v>
+      </c>
     </row>
-    <row r="76" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:88">
       <c r="A76" t="s">
         <v>39</v>
       </c>
@@ -22261,8 +22489,11 @@
       <c r="CI76" s="1">
         <v>139.4</v>
       </c>
+      <c r="CJ76" s="1">
+        <v>134.19999999999999</v>
+      </c>
     </row>
-    <row r="77" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:88">
       <c r="A77" t="s">
         <v>39</v>
       </c>
@@ -22524,8 +22755,11 @@
       <c r="CI77" s="1">
         <v>123.1</v>
       </c>
+      <c r="CJ77" s="1">
+        <v>126.8</v>
+      </c>
     </row>
-    <row r="78" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:88">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -22787,8 +23021,11 @@
       <c r="CI78" s="1">
         <v>115.1</v>
       </c>
+      <c r="CJ78" s="1">
+        <v>109.9</v>
+      </c>
     </row>
-    <row r="79" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:88">
       <c r="A79" t="s">
         <v>39</v>
       </c>
@@ -23050,8 +23287,11 @@
       <c r="CI79" s="1">
         <v>107.2</v>
       </c>
+      <c r="CJ79" s="1">
+        <v>110.9</v>
+      </c>
     </row>
-    <row r="80" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:88">
       <c r="A80" t="s">
         <v>39</v>
       </c>
@@ -23313,8 +23553,11 @@
       <c r="CI80" s="1">
         <v>119.4</v>
       </c>
+      <c r="CJ80" s="1">
+        <v>128.80000000000001</v>
+      </c>
     </row>
-    <row r="81" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:88">
       <c r="A81" t="s">
         <v>39</v>
       </c>
@@ -23576,8 +23819,11 @@
       <c r="CI81" s="1">
         <v>118.3</v>
       </c>
+      <c r="CJ81" s="1">
+        <v>118.7</v>
+      </c>
     </row>
-    <row r="82" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:88">
       <c r="A82" t="s">
         <v>39</v>
       </c>
@@ -23839,8 +24085,11 @@
       <c r="CI82" s="1">
         <v>133.69999999999999</v>
       </c>
+      <c r="CJ82" s="1">
+        <v>144.4</v>
+      </c>
     </row>
-    <row r="83" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:88">
       <c r="A83" t="s">
         <v>39</v>
       </c>
@@ -24102,8 +24351,11 @@
       <c r="CI83" s="1">
         <v>169</v>
       </c>
+      <c r="CJ83" s="1">
+        <v>167.9</v>
+      </c>
     </row>
-    <row r="84" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:88">
       <c r="A84" t="s">
         <v>39</v>
       </c>
@@ -24365,8 +24617,11 @@
       <c r="CI84" s="1">
         <v>131.30000000000001</v>
       </c>
+      <c r="CJ84" s="1">
+        <v>135.9</v>
+      </c>
     </row>
-    <row r="85" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:88">
       <c r="A85" t="s">
         <v>39</v>
       </c>
@@ -24628,8 +24883,11 @@
       <c r="CI85" s="1">
         <v>109.6</v>
       </c>
+      <c r="CJ85" s="1">
+        <v>111.6</v>
+      </c>
     </row>
-    <row r="86" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:88">
       <c r="A86" t="s">
         <v>39</v>
       </c>
@@ -24891,8 +25149,11 @@
       <c r="CI86" s="1">
         <v>123.7</v>
       </c>
+      <c r="CJ86" s="1">
+        <v>123.4</v>
+      </c>
     </row>
-    <row r="87" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:88">
       <c r="A87" t="s">
         <v>39</v>
       </c>
@@ -25154,8 +25415,11 @@
       <c r="CI87" s="1">
         <v>112.3</v>
       </c>
+      <c r="CJ87" s="1">
+        <v>113.5</v>
+      </c>
     </row>
-    <row r="88" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:88">
       <c r="A88" t="s">
         <v>39</v>
       </c>
@@ -25417,8 +25681,11 @@
       <c r="CI88" s="1">
         <v>124.6</v>
       </c>
+      <c r="CJ88" s="1">
+        <v>124.7</v>
+      </c>
     </row>
-    <row r="89" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:88">
       <c r="A89" t="s">
         <v>39</v>
       </c>
@@ -25680,8 +25947,11 @@
       <c r="CI89" s="1">
         <v>118.1</v>
       </c>
+      <c r="CJ89" s="1">
+        <v>118.5</v>
+      </c>
     </row>
-    <row r="90" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:88">
       <c r="A90" t="s">
         <v>39</v>
       </c>
@@ -25943,8 +26213,11 @@
       <c r="CI90" s="1">
         <v>123.9</v>
       </c>
+      <c r="CJ90" s="1">
+        <v>126.4</v>
+      </c>
     </row>
-    <row r="91" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:88">
       <c r="A91" t="s">
         <v>39</v>
       </c>
@@ -26206,8 +26479,11 @@
       <c r="CI91" s="1">
         <v>114.9</v>
       </c>
+      <c r="CJ91" s="1">
+        <v>114.6</v>
+      </c>
     </row>
-    <row r="92" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:88">
       <c r="A92" t="s">
         <v>39</v>
       </c>
@@ -26469,8 +26745,11 @@
       <c r="CI92" s="1">
         <v>126.3</v>
       </c>
+      <c r="CJ92" s="1">
+        <v>128.5</v>
+      </c>
     </row>
-    <row r="93" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:88">
       <c r="A93" t="s">
         <v>39</v>
       </c>
@@ -26732,8 +27011,11 @@
       <c r="CI93" s="1">
         <v>97.8</v>
       </c>
+      <c r="CJ93" s="1">
+        <v>99.9</v>
+      </c>
     </row>
-    <row r="94" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:88">
       <c r="A94" t="s">
         <v>39</v>
       </c>
@@ -26995,8 +27277,11 @@
       <c r="CI94" s="1">
         <v>118.3</v>
       </c>
+      <c r="CJ94" s="1">
+        <v>119.8</v>
+      </c>
     </row>
-    <row r="95" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:88">
       <c r="A95" t="s">
         <v>39</v>
       </c>
@@ -27258,8 +27543,11 @@
       <c r="CI95" s="1">
         <v>120</v>
       </c>
+      <c r="CJ95" s="1">
+        <v>120</v>
+      </c>
     </row>
-    <row r="96" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:88">
       <c r="A96" t="s">
         <v>39</v>
       </c>
@@ -27521,8 +27809,11 @@
       <c r="CI96" s="1">
         <v>114.7</v>
       </c>
+      <c r="CJ96" s="1">
+        <v>115.3</v>
+      </c>
     </row>
-    <row r="97" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:88">
       <c r="A97" t="s">
         <v>39</v>
       </c>
@@ -27784,8 +28075,11 @@
       <c r="CI97" s="1">
         <v>124.5</v>
       </c>
+      <c r="CJ97" s="1">
+        <v>125.3</v>
+      </c>
     </row>
-    <row r="98" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:88">
       <c r="A98" t="s">
         <v>39</v>
       </c>
@@ -28047,8 +28341,11 @@
       <c r="CI98" s="1">
         <v>128.9</v>
       </c>
+      <c r="CJ98" s="1">
+        <v>132.5</v>
+      </c>
     </row>
-    <row r="99" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:88">
       <c r="A99" t="s">
         <v>496</v>
       </c>
@@ -28308,8 +28605,11 @@
       <c r="CI99" s="1">
         <v>115.8</v>
       </c>
+      <c r="CJ99" s="1">
+        <v>115.6</v>
+      </c>
     </row>
-    <row r="100" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:88">
       <c r="A100" t="s">
         <v>39</v>
       </c>
@@ -28571,8 +28871,11 @@
       <c r="CI100" s="1">
         <v>122.1</v>
       </c>
+      <c r="CJ100" s="1">
+        <v>121.3</v>
+      </c>
     </row>
-    <row r="101" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:88">
       <c r="A101" t="s">
         <v>39</v>
       </c>
@@ -28834,8 +29137,11 @@
       <c r="CI101" s="1">
         <v>120.7</v>
       </c>
+      <c r="CJ101" s="1">
+        <v>121.4</v>
+      </c>
     </row>
-    <row r="102" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:88">
       <c r="A102" t="s">
         <v>39</v>
       </c>
@@ -29097,8 +29403,11 @@
       <c r="CI102" s="1">
         <v>122.5</v>
       </c>
+      <c r="CJ102" s="1">
+        <v>122.9</v>
+      </c>
     </row>
-    <row r="103" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:88">
       <c r="A103" t="s">
         <v>39</v>
       </c>
@@ -29360,8 +29669,11 @@
       <c r="CI103" s="1">
         <v>117.3</v>
       </c>
+      <c r="CJ103" s="1">
+        <v>118.5</v>
+      </c>
     </row>
-    <row r="104" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:88">
       <c r="A104" t="s">
         <v>39</v>
       </c>
@@ -29623,8 +29935,11 @@
       <c r="CI104" s="1">
         <v>134.5</v>
       </c>
+      <c r="CJ104" s="1">
+        <v>136.5</v>
+      </c>
     </row>
-    <row r="105" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:88">
       <c r="A105" t="s">
         <v>39</v>
       </c>
@@ -29886,8 +30201,11 @@
       <c r="CI105" s="1">
         <v>126.1</v>
       </c>
+      <c r="CJ105" s="1">
+        <v>127.4</v>
+      </c>
     </row>
-    <row r="106" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:88">
       <c r="A106" t="s">
         <v>39</v>
       </c>
@@ -30149,8 +30467,11 @@
       <c r="CI106" s="1">
         <v>119.9</v>
       </c>
+      <c r="CJ106" s="1">
+        <v>120.6</v>
+      </c>
     </row>
-    <row r="107" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:88">
       <c r="A107" t="s">
         <v>39</v>
       </c>
@@ -30412,8 +30733,11 @@
       <c r="CI107" s="1">
         <v>123.6</v>
       </c>
+      <c r="CJ107" s="1">
+        <v>123.3</v>
+      </c>
     </row>
-    <row r="108" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:88">
       <c r="A108" t="s">
         <v>39</v>
       </c>
@@ -30675,8 +30999,11 @@
       <c r="CI108" s="1">
         <v>121.1</v>
       </c>
+      <c r="CJ108" s="1">
+        <v>119.4</v>
+      </c>
     </row>
-    <row r="109" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:88">
       <c r="A109" t="s">
         <v>39</v>
       </c>
@@ -30938,8 +31265,11 @@
       <c r="CI109" s="1">
         <v>116.9</v>
       </c>
+      <c r="CJ109" s="1">
+        <v>117</v>
+      </c>
     </row>
-    <row r="110" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:88">
       <c r="A110" t="s">
         <v>39</v>
       </c>
@@ -31201,8 +31531,11 @@
       <c r="CI110" s="1">
         <v>112.2</v>
       </c>
+      <c r="CJ110" s="1">
+        <v>112.6</v>
+      </c>
     </row>
-    <row r="111" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:88">
       <c r="A111" t="s">
         <v>39</v>
       </c>
@@ -31464,8 +31797,11 @@
       <c r="CI111" s="1">
         <v>109.6</v>
       </c>
+      <c r="CJ111" s="1">
+        <v>110.5</v>
+      </c>
     </row>
-    <row r="112" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:88">
       <c r="A112" t="s">
         <v>39</v>
       </c>
@@ -31727,8 +32063,11 @@
       <c r="CI112" s="1">
         <v>112.9</v>
       </c>
+      <c r="CJ112" s="1">
+        <v>113.5</v>
+      </c>
     </row>
-    <row r="113" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:88">
       <c r="A113" t="s">
         <v>39</v>
       </c>
@@ -31990,8 +32329,11 @@
       <c r="CI113" s="1">
         <v>118</v>
       </c>
+      <c r="CJ113" s="1">
+        <v>121.9</v>
+      </c>
     </row>
-    <row r="114" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:88">
       <c r="A114" t="s">
         <v>39</v>
       </c>
@@ -32253,8 +32595,11 @@
       <c r="CI114" s="1">
         <v>130.69999999999999</v>
       </c>
+      <c r="CJ114" s="1">
+        <v>132.19999999999999</v>
+      </c>
     </row>
-    <row r="115" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:88">
       <c r="A115" t="s">
         <v>39</v>
       </c>
@@ -32516,8 +32861,11 @@
       <c r="CI115" s="1">
         <v>119.1</v>
       </c>
+      <c r="CJ115" s="1">
+        <v>119</v>
+      </c>
     </row>
-    <row r="116" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:88">
       <c r="A116" t="s">
         <v>39</v>
       </c>
@@ -32779,8 +33127,11 @@
       <c r="CI116" s="1">
         <v>115.1</v>
       </c>
+      <c r="CJ116" s="1">
+        <v>115.2</v>
+      </c>
     </row>
-    <row r="117" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:88">
       <c r="A117" t="s">
         <v>39</v>
       </c>
@@ -33042,8 +33393,11 @@
       <c r="CI117" s="1">
         <v>127.2</v>
       </c>
+      <c r="CJ117" s="1">
+        <v>127.6</v>
+      </c>
     </row>
-    <row r="118" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:88">
       <c r="A118" t="s">
         <v>39</v>
       </c>
@@ -33305,8 +33659,11 @@
       <c r="CI118" s="1">
         <v>119.8</v>
       </c>
+      <c r="CJ118" s="1">
+        <v>119.8</v>
+      </c>
     </row>
-    <row r="119" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:88">
       <c r="A119" t="s">
         <v>39</v>
       </c>
@@ -33568,8 +33925,11 @@
       <c r="CI119" s="1">
         <v>127.4</v>
       </c>
+      <c r="CJ119" s="1">
+        <v>128.19999999999999</v>
+      </c>
     </row>
-    <row r="120" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:88">
       <c r="A120" t="s">
         <v>39</v>
       </c>
@@ -33831,8 +34191,11 @@
       <c r="CI120" s="1">
         <v>125.7</v>
       </c>
+      <c r="CJ120" s="1">
+        <v>126.8</v>
+      </c>
     </row>
-    <row r="121" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:88">
       <c r="A121" t="s">
         <v>39</v>
       </c>
@@ -34094,8 +34457,11 @@
       <c r="CI121" s="1">
         <v>120</v>
       </c>
+      <c r="CJ121" s="1">
+        <v>121</v>
+      </c>
     </row>
-    <row r="122" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:88">
       <c r="A122" t="s">
         <v>39</v>
       </c>
@@ -34357,8 +34723,11 @@
       <c r="CI122" s="1">
         <v>109.3</v>
       </c>
+      <c r="CJ122" s="1">
+        <v>111</v>
+      </c>
     </row>
-    <row r="123" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:88">
       <c r="A123" t="s">
         <v>39</v>
       </c>
@@ -34620,8 +34989,11 @@
       <c r="CI123" s="1">
         <v>104.7</v>
       </c>
+      <c r="CJ123" s="1">
+        <v>104.3</v>
+      </c>
     </row>
-    <row r="124" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:88">
       <c r="A124" t="s">
         <v>39</v>
       </c>
@@ -34883,8 +35255,11 @@
       <c r="CI124" s="1">
         <v>115.9</v>
       </c>
+      <c r="CJ124" s="1">
+        <v>119.6</v>
+      </c>
     </row>
-    <row r="125" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:88">
       <c r="A125" t="s">
         <v>39</v>
       </c>
@@ -35146,8 +35521,11 @@
       <c r="CI125" s="1">
         <v>118.5</v>
       </c>
+      <c r="CJ125" s="1">
+        <v>119</v>
+      </c>
     </row>
-    <row r="126" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:88">
       <c r="A126" t="s">
         <v>39</v>
       </c>
@@ -35409,8 +35787,11 @@
       <c r="CI126" s="1">
         <v>110.8</v>
       </c>
+      <c r="CJ126" s="1">
+        <v>110.9</v>
+      </c>
     </row>
-    <row r="127" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:88">
       <c r="A127" t="s">
         <v>39</v>
       </c>
@@ -35672,8 +36053,11 @@
       <c r="CI127" s="1">
         <v>110.1</v>
       </c>
+      <c r="CJ127" s="1">
+        <v>109.9</v>
+      </c>
     </row>
-    <row r="128" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:88">
       <c r="A128" t="s">
         <v>39</v>
       </c>
@@ -35935,8 +36319,11 @@
       <c r="CI128" s="1">
         <v>112</v>
       </c>
+      <c r="CJ128" s="1">
+        <v>111.4</v>
+      </c>
     </row>
-    <row r="129" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:88">
       <c r="A129" t="s">
         <v>39</v>
       </c>
@@ -36198,8 +36585,11 @@
       <c r="CI129" s="1">
         <v>121.2</v>
       </c>
+      <c r="CJ129" s="1">
+        <v>123.5</v>
+      </c>
     </row>
-    <row r="130" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:88">
       <c r="A130" t="s">
         <v>39</v>
       </c>
@@ -36461,8 +36851,11 @@
       <c r="CI130" s="1">
         <v>110.3</v>
       </c>
+      <c r="CJ130" s="1">
+        <v>111.8</v>
+      </c>
     </row>
-    <row r="131" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:88">
       <c r="A131" t="s">
         <v>39</v>
       </c>
@@ -36724,8 +37117,11 @@
       <c r="CI131" s="1">
         <v>124.3</v>
       </c>
+      <c r="CJ131" s="1">
+        <v>124.3</v>
+      </c>
     </row>
-    <row r="132" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:88">
       <c r="A132" t="s">
         <v>39</v>
       </c>
@@ -36987,8 +37383,11 @@
       <c r="CI132" s="1">
         <v>108.8</v>
       </c>
+      <c r="CJ132" s="1">
+        <v>108.8</v>
+      </c>
     </row>
-    <row r="133" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:88">
       <c r="A133" t="s">
         <v>39</v>
       </c>
@@ -37250,8 +37649,11 @@
       <c r="CI133" s="1">
         <v>118.7</v>
       </c>
+      <c r="CJ133" s="1">
+        <v>119.3</v>
+      </c>
     </row>
-    <row r="134" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:88">
       <c r="A134" t="s">
         <v>39</v>
       </c>
@@ -37513,8 +37915,11 @@
       <c r="CI134" s="1">
         <v>105.4</v>
       </c>
+      <c r="CJ134" s="1">
+        <v>104.4</v>
+      </c>
     </row>
-    <row r="135" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:88">
       <c r="A135" t="s">
         <v>39</v>
       </c>
@@ -37776,8 +38181,11 @@
       <c r="CI135" s="1">
         <v>117.6</v>
       </c>
+      <c r="CJ135" s="1">
+        <v>117.4</v>
+      </c>
     </row>
-    <row r="136" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:88">
       <c r="A136" t="s">
         <v>39</v>
       </c>
@@ -38039,8 +38447,11 @@
       <c r="CI136" s="1">
         <v>110.7</v>
       </c>
+      <c r="CJ136" s="1">
+        <v>110.4</v>
+      </c>
     </row>
-    <row r="137" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:88">
       <c r="A137" t="s">
         <v>39</v>
       </c>
@@ -38302,8 +38713,11 @@
       <c r="CI137" s="1">
         <v>113.5</v>
       </c>
+      <c r="CJ137" s="1">
+        <v>113.5</v>
+      </c>
     </row>
-    <row r="138" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:88">
       <c r="A138" t="s">
         <v>39</v>
       </c>
@@ -38565,8 +38979,11 @@
       <c r="CI138" s="1">
         <v>114.6</v>
       </c>
+      <c r="CJ138" s="1">
+        <v>114.2</v>
+      </c>
     </row>
-    <row r="139" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:88">
       <c r="A139" t="s">
         <v>39</v>
       </c>
@@ -38828,8 +39245,11 @@
       <c r="CI139" s="1">
         <v>111.6</v>
       </c>
+      <c r="CJ139" s="1">
+        <v>111.3</v>
+      </c>
     </row>
-    <row r="140" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:88">
       <c r="A140" t="s">
         <v>39</v>
       </c>
@@ -39091,8 +39511,11 @@
       <c r="CI140" s="1">
         <v>111.2</v>
       </c>
+      <c r="CJ140" s="1">
+        <v>110.3</v>
+      </c>
     </row>
-    <row r="141" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:88">
       <c r="A141" t="s">
         <v>39</v>
       </c>
@@ -39354,8 +39777,11 @@
       <c r="CI141" s="1">
         <v>109.4</v>
       </c>
+      <c r="CJ141" s="1">
+        <v>109.4</v>
+      </c>
     </row>
-    <row r="142" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:88">
       <c r="A142" t="s">
         <v>39</v>
       </c>
@@ -39617,8 +40043,11 @@
       <c r="CI142" s="1">
         <v>110.3</v>
       </c>
+      <c r="CJ142" s="1">
+        <v>111</v>
+      </c>
     </row>
-    <row r="143" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:88">
       <c r="A143" t="s">
         <v>39</v>
       </c>
@@ -39880,8 +40309,11 @@
       <c r="CI143" s="1">
         <v>106.9</v>
       </c>
+      <c r="CJ143" s="1">
+        <v>107.2</v>
+      </c>
     </row>
-    <row r="144" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:88">
       <c r="A144" t="s">
         <v>39</v>
       </c>
@@ -40143,8 +40575,11 @@
       <c r="CI144" s="1">
         <v>103</v>
       </c>
+      <c r="CJ144" s="1">
+        <v>102.2</v>
+      </c>
     </row>
-    <row r="145" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:88">
       <c r="A145" t="s">
         <v>39</v>
       </c>
@@ -40406,8 +40841,11 @@
       <c r="CI145" s="1">
         <v>104.3</v>
       </c>
+      <c r="CJ145" s="1">
+        <v>105.1</v>
+      </c>
     </row>
-    <row r="146" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:88">
       <c r="A146" t="s">
         <v>39</v>
       </c>
@@ -40669,8 +41107,11 @@
       <c r="CI146" s="1">
         <v>103</v>
       </c>
+      <c r="CJ146" s="1">
+        <v>103.1</v>
+      </c>
     </row>
-    <row r="147" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:88">
       <c r="A147" t="s">
         <v>39</v>
       </c>
@@ -40932,8 +41373,11 @@
       <c r="CI147" s="1">
         <v>103.5</v>
       </c>
+      <c r="CJ147" s="1">
+        <v>103.6</v>
+      </c>
     </row>
-    <row r="148" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:88">
       <c r="A148" t="s">
         <v>39</v>
       </c>
@@ -41195,8 +41639,11 @@
       <c r="CI148" s="1">
         <v>104.7</v>
       </c>
+      <c r="CJ148" s="1">
+        <v>105.3</v>
+      </c>
     </row>
-    <row r="149" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:88">
       <c r="A149" t="s">
         <v>39</v>
       </c>
@@ -41458,8 +41905,11 @@
       <c r="CI149" s="1">
         <v>104.1</v>
       </c>
+      <c r="CJ149" s="1">
+        <v>104.1</v>
+      </c>
     </row>
-    <row r="150" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:88">
       <c r="A150" t="s">
         <v>39</v>
       </c>
@@ -41721,8 +42171,11 @@
       <c r="CI150" s="1">
         <v>104.4</v>
       </c>
+      <c r="CJ150" s="1">
+        <v>104.4</v>
+      </c>
     </row>
-    <row r="151" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:88">
       <c r="A151" t="s">
         <v>39</v>
       </c>
@@ -41984,8 +42437,11 @@
       <c r="CI151" s="1">
         <v>103.7</v>
       </c>
+      <c r="CJ151" s="1">
+        <v>103.7</v>
+      </c>
     </row>
-    <row r="152" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:88">
       <c r="A152" t="s">
         <v>39</v>
       </c>
@@ -42247,8 +42703,11 @@
       <c r="CI152" s="1">
         <v>103.8</v>
       </c>
+      <c r="CJ152" s="1">
+        <v>103.8</v>
+      </c>
     </row>
-    <row r="153" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:88">
       <c r="A153" t="s">
         <v>39</v>
       </c>
@@ -42510,8 +42969,11 @@
       <c r="CI153" s="1">
         <v>104.5</v>
       </c>
+      <c r="CJ153" s="1">
+        <v>104.5</v>
+      </c>
     </row>
-    <row r="154" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:88">
       <c r="A154" t="s">
         <v>39</v>
       </c>
@@ -42773,8 +43235,11 @@
       <c r="CI154" s="1">
         <v>104.5</v>
       </c>
+      <c r="CJ154" s="1">
+        <v>104.5</v>
+      </c>
     </row>
-    <row r="155" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:88">
       <c r="A155" t="s">
         <v>39</v>
       </c>
@@ -43036,8 +43501,11 @@
       <c r="CI155" s="1">
         <v>103.8</v>
       </c>
+      <c r="CJ155" s="1">
+        <v>103.8</v>
+      </c>
     </row>
-    <row r="156" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:88">
       <c r="A156" t="s">
         <v>39</v>
       </c>
@@ -43299,8 +43767,11 @@
       <c r="CI156" s="1">
         <v>104.5</v>
       </c>
+      <c r="CJ156" s="1">
+        <v>104.5</v>
+      </c>
     </row>
-    <row r="157" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:88">
       <c r="A157" t="s">
         <v>39</v>
       </c>
@@ -43562,8 +44033,11 @@
       <c r="CI157" s="1">
         <v>113.3</v>
       </c>
+      <c r="CJ157" s="1">
+        <v>113.4</v>
+      </c>
     </row>
-    <row r="158" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:88">
       <c r="A158" t="s">
         <v>39</v>
       </c>
@@ -43825,8 +44299,11 @@
       <c r="CI158" s="1">
         <v>104.3</v>
       </c>
+      <c r="CJ158" s="1">
+        <v>104.3</v>
+      </c>
     </row>
-    <row r="159" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:88">
       <c r="A159" t="s">
         <v>39</v>
       </c>
@@ -44088,8 +44565,11 @@
       <c r="CI159" s="1">
         <v>118.5</v>
       </c>
+      <c r="CJ159" s="1">
+        <v>118.5</v>
+      </c>
     </row>
-    <row r="160" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:88">
       <c r="A160" t="s">
         <v>39</v>
       </c>
@@ -44351,8 +44831,11 @@
       <c r="CI160" s="1">
         <v>106.7</v>
       </c>
+      <c r="CJ160" s="1">
+        <v>110.8</v>
+      </c>
     </row>
-    <row r="161" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:88">
       <c r="A161" t="s">
         <v>39</v>
       </c>
@@ -44614,8 +45097,11 @@
       <c r="CI161" s="1">
         <v>123.5</v>
       </c>
+      <c r="CJ161" s="1">
+        <v>124.4</v>
+      </c>
     </row>
-    <row r="162" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:88">
       <c r="A162" t="s">
         <v>39</v>
       </c>
@@ -44877,8 +45363,11 @@
       <c r="CI162" s="1">
         <v>137.80000000000001</v>
       </c>
+      <c r="CJ162" s="1">
+        <v>140.9</v>
+      </c>
     </row>
-    <row r="163" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:88">
       <c r="A163" t="s">
         <v>39</v>
       </c>
@@ -45140,8 +45629,11 @@
       <c r="CI163" s="1">
         <v>101.2</v>
       </c>
+      <c r="CJ163" s="1">
+        <v>100.5</v>
+      </c>
     </row>
-    <row r="164" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:88">
       <c r="A164" t="s">
         <v>39</v>
       </c>
@@ -45403,8 +45895,11 @@
       <c r="CI164" s="1">
         <v>103</v>
       </c>
+      <c r="CJ164" s="1">
+        <v>103.5</v>
+      </c>
     </row>
-    <row r="165" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:88">
       <c r="A165" t="s">
         <v>39</v>
       </c>
@@ -45666,8 +46161,11 @@
       <c r="CI165" s="1">
         <v>106.7</v>
       </c>
+      <c r="CJ165" s="1">
+        <v>105.5</v>
+      </c>
     </row>
-    <row r="166" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:88">
       <c r="A166" t="s">
         <v>39</v>
       </c>
@@ -45929,8 +46427,11 @@
       <c r="CI166" s="1">
         <v>110.4</v>
       </c>
+      <c r="CJ166" s="1">
+        <v>109.4</v>
+      </c>
     </row>
-    <row r="167" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:88">
       <c r="A167" t="s">
         <v>39</v>
       </c>
@@ -46192,8 +46693,11 @@
       <c r="CI167" s="1">
         <v>107.1</v>
       </c>
+      <c r="CJ167" s="1">
+        <v>107.3</v>
+      </c>
     </row>
-    <row r="168" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:88">
       <c r="A168" t="s">
         <v>39</v>
       </c>
@@ -46455,8 +46959,11 @@
       <c r="CI168" s="1">
         <v>108.7</v>
       </c>
+      <c r="CJ168" s="1">
+        <v>108.2</v>
+      </c>
     </row>
-    <row r="169" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:88">
       <c r="A169" t="s">
         <v>39</v>
       </c>
@@ -46718,8 +47225,11 @@
       <c r="CI169" s="1">
         <v>106</v>
       </c>
+      <c r="CJ169" s="1">
+        <v>103.7</v>
+      </c>
     </row>
-    <row r="170" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:88">
       <c r="A170" t="s">
         <v>39</v>
       </c>
@@ -46981,8 +47491,11 @@
       <c r="CI170" s="1">
         <v>109.3</v>
       </c>
+      <c r="CJ170" s="1">
+        <v>110.1</v>
+      </c>
     </row>
-    <row r="171" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:88">
       <c r="A171" t="s">
         <v>39</v>
       </c>
@@ -47244,8 +47757,11 @@
       <c r="CI171" s="1">
         <v>108.5</v>
       </c>
+      <c r="CJ171" s="1">
+        <v>109.6</v>
+      </c>
     </row>
-    <row r="172" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:88">
       <c r="A172" t="s">
         <v>39</v>
       </c>
@@ -47507,8 +48023,11 @@
       <c r="CI172" s="1">
         <v>107.8</v>
       </c>
+      <c r="CJ172" s="1">
+        <v>109.1</v>
+      </c>
     </row>
-    <row r="173" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:88">
       <c r="A173" t="s">
         <v>39</v>
       </c>
@@ -47770,8 +48289,11 @@
       <c r="CI173" s="1">
         <v>110</v>
       </c>
+      <c r="CJ173" s="1">
+        <v>110</v>
+      </c>
     </row>
-    <row r="174" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:88">
       <c r="A174" t="s">
         <v>39</v>
       </c>
@@ -48033,8 +48555,11 @@
       <c r="CI174" s="1">
         <v>132.4</v>
       </c>
+      <c r="CJ174" s="1">
+        <v>132.9</v>
+      </c>
     </row>
-    <row r="175" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:88">
       <c r="A175" t="s">
         <v>39</v>
       </c>
@@ -48296,8 +48821,11 @@
       <c r="CI175" s="1">
         <v>106.8</v>
       </c>
+      <c r="CJ175" s="1">
+        <v>106.8</v>
+      </c>
     </row>
-    <row r="176" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:88">
       <c r="A176" t="s">
         <v>39</v>
       </c>
@@ -48559,8 +49087,11 @@
       <c r="CI176" s="1">
         <v>110</v>
       </c>
+      <c r="CJ176" s="1">
+        <v>110.2</v>
+      </c>
     </row>
-    <row r="177" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:88">
       <c r="A177" t="s">
         <v>39</v>
       </c>
@@ -48822,8 +49353,11 @@
       <c r="CI177" s="1">
         <v>111.2</v>
       </c>
+      <c r="CJ177" s="1">
+        <v>111.2</v>
+      </c>
     </row>
-    <row r="178" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:88">
       <c r="A178" t="s">
         <v>39</v>
       </c>
@@ -49085,8 +49619,11 @@
       <c r="CI178" s="1">
         <v>110.3</v>
       </c>
+      <c r="CJ178" s="1">
+        <v>110.3</v>
+      </c>
     </row>
-    <row r="179" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:88">
       <c r="A179" t="s">
         <v>39</v>
       </c>
@@ -49348,8 +49885,11 @@
       <c r="CI179" s="1">
         <v>109</v>
       </c>
+      <c r="CJ179" s="1">
+        <v>109</v>
+      </c>
     </row>
-    <row r="180" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:88">
       <c r="A180" t="s">
         <v>39</v>
       </c>
@@ -49611,8 +50151,11 @@
       <c r="CI180" s="1">
         <v>112.1</v>
       </c>
+      <c r="CJ180" s="1">
+        <v>112.5</v>
+      </c>
     </row>
-    <row r="181" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:88">
       <c r="A181" t="s">
         <v>39</v>
       </c>
@@ -49874,8 +50417,11 @@
       <c r="CI181" s="1">
         <v>120.8</v>
       </c>
+      <c r="CJ181" s="1">
+        <v>121.5</v>
+      </c>
     </row>
-    <row r="182" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:88">
       <c r="A182" t="s">
         <v>39</v>
       </c>
@@ -50137,8 +50683,11 @@
       <c r="CI182" s="1">
         <v>117</v>
       </c>
+      <c r="CJ182" s="1">
+        <v>119.5</v>
+      </c>
     </row>
-    <row r="183" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:88">
       <c r="A183" t="s">
         <v>39</v>
       </c>
@@ -50400,8 +50949,11 @@
       <c r="CI183" s="1">
         <v>111.2</v>
       </c>
+      <c r="CJ183" s="1">
+        <v>113.6</v>
+      </c>
     </row>
-    <row r="184" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:88">
       <c r="A184" t="s">
         <v>496</v>
       </c>
@@ -50663,8 +51215,11 @@
       <c r="CI184" s="1">
         <v>110.4</v>
       </c>
+      <c r="CJ184" s="1">
+        <v>112.2</v>
+      </c>
     </row>
-    <row r="185" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:88">
       <c r="A185" t="s">
         <v>497</v>
       </c>
@@ -50926,8 +51481,11 @@
       <c r="CI185" s="1">
         <v>113.3</v>
       </c>
+      <c r="CJ185" s="1">
+        <v>117</v>
+      </c>
     </row>
-    <row r="186" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:88">
       <c r="A186" t="s">
         <v>39</v>
       </c>
@@ -51189,8 +51747,11 @@
       <c r="CI186" s="1">
         <v>114.6</v>
       </c>
+      <c r="CJ186" s="1">
+        <v>114.9</v>
+      </c>
     </row>
-    <row r="187" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:88">
       <c r="A187" t="s">
         <v>39</v>
       </c>
@@ -51452,8 +52013,11 @@
       <c r="CI187" s="1">
         <v>105.2</v>
       </c>
+      <c r="CJ187" s="1">
+        <v>105.3</v>
+      </c>
     </row>
-    <row r="188" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:88">
       <c r="A188" t="s">
         <v>39</v>
       </c>
@@ -51715,8 +52279,11 @@
       <c r="CI188" s="1">
         <v>106.2</v>
       </c>
+      <c r="CJ188" s="1">
+        <v>106.2</v>
+      </c>
     </row>
-    <row r="189" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:88">
       <c r="A189" t="s">
         <v>39</v>
       </c>
@@ -51978,8 +52545,11 @@
       <c r="CI189" s="1">
         <v>115.6</v>
       </c>
+      <c r="CJ189" s="1">
+        <v>115.4</v>
+      </c>
     </row>
-    <row r="190" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:88">
       <c r="A190" t="s">
         <v>39</v>
       </c>
@@ -52241,8 +52811,11 @@
       <c r="CI190" s="1">
         <v>112.1</v>
       </c>
+      <c r="CJ190" s="1">
+        <v>114</v>
+      </c>
     </row>
-    <row r="191" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:88">
       <c r="A191" t="s">
         <v>39</v>
       </c>
@@ -52504,8 +53077,11 @@
       <c r="CI191" s="1">
         <v>105</v>
       </c>
+      <c r="CJ191" s="1">
+        <v>105</v>
+      </c>
     </row>
-    <row r="192" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:88">
       <c r="A192" t="s">
         <v>39</v>
       </c>
@@ -52767,8 +53343,11 @@
       <c r="CI192" s="1">
         <v>90.8</v>
       </c>
+      <c r="CJ192" s="1">
+        <v>90.7</v>
+      </c>
     </row>
-    <row r="193" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:88">
       <c r="A193" t="s">
         <v>39</v>
       </c>
@@ -53030,8 +53609,11 @@
       <c r="CI193" s="1">
         <v>100.2</v>
       </c>
+      <c r="CJ193" s="1">
+        <v>100.2</v>
+      </c>
     </row>
-    <row r="194" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:88">
       <c r="A194" t="s">
         <v>39</v>
       </c>
@@ -53293,8 +53875,11 @@
       <c r="CI194" s="1">
         <v>98.2</v>
       </c>
+      <c r="CJ194" s="1">
+        <v>98</v>
+      </c>
     </row>
-    <row r="195" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:88">
       <c r="A195" t="s">
         <v>39</v>
       </c>
@@ -53556,8 +54141,11 @@
       <c r="CI195" s="1">
         <v>86.6</v>
       </c>
+      <c r="CJ195" s="1">
+        <v>87.2</v>
+      </c>
     </row>
-    <row r="196" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:88">
       <c r="A196" t="s">
         <v>39</v>
       </c>
@@ -53819,8 +54407,11 @@
       <c r="CI196" s="1">
         <v>107.5</v>
       </c>
+      <c r="CJ196" s="1">
+        <v>106.2</v>
+      </c>
     </row>
-    <row r="197" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:88">
       <c r="A197" t="s">
         <v>39</v>
       </c>
@@ -54082,8 +54673,11 @@
       <c r="CI197" s="1">
         <v>93</v>
       </c>
+      <c r="CJ197" s="1">
+        <v>92.6</v>
+      </c>
     </row>
-    <row r="198" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:88">
       <c r="A198" t="s">
         <v>39</v>
       </c>
@@ -54345,8 +54939,11 @@
       <c r="CI198" s="1">
         <v>98.7</v>
       </c>
+      <c r="CJ198" s="1">
+        <v>98.5</v>
+      </c>
     </row>
-    <row r="199" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:88">
       <c r="A199" t="s">
         <v>39</v>
       </c>
@@ -54608,8 +55205,11 @@
       <c r="CI199" s="1">
         <v>119.8</v>
       </c>
+      <c r="CJ199" s="1">
+        <v>120.8</v>
+      </c>
     </row>
-    <row r="200" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:88">
       <c r="A200" t="s">
         <v>39</v>
       </c>
@@ -54871,8 +55471,11 @@
       <c r="CI200" s="1">
         <v>99</v>
       </c>
+      <c r="CJ200" s="1">
+        <v>101.5</v>
+      </c>
     </row>
-    <row r="201" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:88">
       <c r="A201" t="s">
         <v>39</v>
       </c>
@@ -55134,8 +55737,11 @@
       <c r="CI201" s="1">
         <v>119.9</v>
       </c>
+      <c r="CJ201" s="1">
+        <v>120.9</v>
+      </c>
     </row>
-    <row r="202" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:88">
       <c r="A202" t="s">
         <v>39</v>
       </c>
@@ -55397,8 +56003,11 @@
       <c r="CI202" s="1">
         <v>112.9</v>
       </c>
+      <c r="CJ202" s="1">
+        <v>114.6</v>
+      </c>
     </row>
-    <row r="203" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:88">
       <c r="A203" t="s">
         <v>39</v>
       </c>
@@ -55660,8 +56269,11 @@
       <c r="CI203" s="1">
         <v>117.8</v>
       </c>
+      <c r="CJ203" s="1">
+        <v>118.8</v>
+      </c>
     </row>
-    <row r="204" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:88">
       <c r="A204" t="s">
         <v>39</v>
       </c>
@@ -55923,8 +56535,11 @@
       <c r="CI204" s="1">
         <v>100.5</v>
       </c>
+      <c r="CJ204" s="1">
+        <v>100.6</v>
+      </c>
     </row>
-    <row r="205" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:88">
       <c r="A205" t="s">
         <v>39</v>
       </c>
@@ -56186,8 +56801,11 @@
       <c r="CI205" s="1">
         <v>114.7</v>
       </c>
+      <c r="CJ205" s="1">
+        <v>114.7</v>
+      </c>
     </row>
-    <row r="206" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:88">
       <c r="A206" t="s">
         <v>39</v>
       </c>
@@ -56449,8 +57067,11 @@
       <c r="CI206" s="1">
         <v>108.8</v>
       </c>
+      <c r="CJ206" s="1">
+        <v>108.8</v>
+      </c>
     </row>
-    <row r="207" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:88">
       <c r="A207" t="s">
         <v>39</v>
       </c>
@@ -56712,8 +57333,11 @@
       <c r="CI207" s="1">
         <v>100</v>
       </c>
+      <c r="CJ207" s="1">
+        <v>100</v>
+      </c>
     </row>
-    <row r="208" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:88">
       <c r="A208" t="s">
         <v>39</v>
       </c>
@@ -56975,8 +57599,11 @@
       <c r="CI208" s="1">
         <v>106.7</v>
       </c>
+      <c r="CJ208" s="1">
+        <v>108.9</v>
+      </c>
     </row>
-    <row r="209" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:88">
       <c r="A209" t="s">
         <v>39</v>
       </c>
@@ -57238,8 +57865,11 @@
       <c r="CI209" s="1">
         <v>122.6</v>
       </c>
+      <c r="CJ209" s="1">
+        <v>122.6</v>
+      </c>
     </row>
-    <row r="210" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:88">
       <c r="A210" t="s">
         <v>39</v>
       </c>
@@ -57501,8 +58131,11 @@
       <c r="CI210" s="1">
         <v>115.5</v>
       </c>
+      <c r="CJ210" s="1">
+        <v>117.1</v>
+      </c>
     </row>
-    <row r="211" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:88">
       <c r="A211" t="s">
         <v>39</v>
       </c>
@@ -57764,8 +58397,11 @@
       <c r="CI211" s="1">
         <v>109.6</v>
       </c>
+      <c r="CJ211" s="1">
+        <v>110.3</v>
+      </c>
     </row>
-    <row r="212" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:88">
       <c r="A212" t="s">
         <v>39</v>
       </c>
@@ -58027,8 +58663,11 @@
       <c r="CI212" s="1">
         <v>110.9</v>
       </c>
+      <c r="CJ212" s="1">
+        <v>110.9</v>
+      </c>
     </row>
-    <row r="213" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:88">
       <c r="A213" t="s">
         <v>39</v>
       </c>
@@ -58290,8 +58929,11 @@
       <c r="CI213" s="1">
         <v>110.8</v>
       </c>
+      <c r="CJ213" s="1">
+        <v>110.8</v>
+      </c>
     </row>
-    <row r="214" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:88">
       <c r="A214" t="s">
         <v>39</v>
       </c>
@@ -58553,8 +59195,11 @@
       <c r="CI214" s="1">
         <v>109.7</v>
       </c>
+      <c r="CJ214" s="1">
+        <v>109.7</v>
+      </c>
     </row>
-    <row r="215" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:88">
       <c r="A215" t="s">
         <v>39</v>
       </c>
@@ -58816,8 +59461,11 @@
       <c r="CI215" s="1">
         <v>111.5</v>
       </c>
+      <c r="CJ215" s="1">
+        <v>112.5</v>
+      </c>
     </row>
-    <row r="216" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:88">
       <c r="A216" t="s">
         <v>39</v>
       </c>
@@ -59079,8 +59727,11 @@
       <c r="CI216" s="1">
         <v>106.8</v>
       </c>
+      <c r="CJ216" s="1">
+        <v>108</v>
+      </c>
     </row>
-    <row r="217" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:88">
       <c r="A217" t="s">
         <v>39</v>
       </c>
@@ -59342,8 +59993,11 @@
       <c r="CI217" s="1">
         <v>123.4</v>
       </c>
+      <c r="CJ217" s="1">
+        <v>123.5</v>
+      </c>
     </row>
-    <row r="218" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:88">
       <c r="A218" t="s">
         <v>39</v>
       </c>
@@ -59605,8 +60259,11 @@
       <c r="CI218" s="1">
         <v>97.3</v>
       </c>
+      <c r="CJ218" s="1">
+        <v>96.1</v>
+      </c>
     </row>
-    <row r="219" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:88">
       <c r="A219" t="s">
         <v>39</v>
       </c>
@@ -59868,8 +60525,11 @@
       <c r="CI219" s="1">
         <v>109.1</v>
       </c>
+      <c r="CJ219" s="1">
+        <v>109</v>
+      </c>
     </row>
-    <row r="220" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:88">
       <c r="A220" t="s">
         <v>39</v>
       </c>
@@ -60131,8 +60791,11 @@
       <c r="CI220" s="1">
         <v>97.7</v>
       </c>
+      <c r="CJ220" s="1">
+        <v>100.2</v>
+      </c>
     </row>
-    <row r="221" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:88">
       <c r="A221" t="s">
         <v>39</v>
       </c>
@@ -60394,8 +61057,11 @@
       <c r="CI221" s="1">
         <v>110.7</v>
       </c>
+      <c r="CJ221" s="1">
+        <v>110.7</v>
+      </c>
     </row>
-    <row r="222" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:88">
       <c r="A222" t="s">
         <v>39</v>
       </c>
@@ -60657,8 +61323,11 @@
       <c r="CI222" s="1">
         <v>103</v>
       </c>
+      <c r="CJ222" s="1">
+        <v>103</v>
+      </c>
     </row>
-    <row r="223" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:88">
       <c r="A223" t="s">
         <v>39</v>
       </c>
@@ -60920,8 +61589,11 @@
       <c r="CI223" s="1">
         <v>112</v>
       </c>
+      <c r="CJ223" s="1">
+        <v>112</v>
+      </c>
     </row>
-    <row r="224" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:88">
       <c r="A224" t="s">
         <v>39</v>
       </c>
@@ -61183,8 +61855,11 @@
       <c r="CI224" s="1">
         <v>101.9</v>
       </c>
+      <c r="CJ224" s="1">
+        <v>101.9</v>
+      </c>
     </row>
-    <row r="225" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:88">
       <c r="A225" t="s">
         <v>39</v>
       </c>
@@ -61446,8 +62121,11 @@
       <c r="CI225" s="1">
         <v>107.1</v>
       </c>
+      <c r="CJ225" s="1">
+        <v>107.1</v>
+      </c>
     </row>
-    <row r="226" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:88">
       <c r="A226" t="s">
         <v>39</v>
       </c>
@@ -61709,8 +62387,11 @@
       <c r="CI226" s="1">
         <v>105.9</v>
       </c>
+      <c r="CJ226" s="1">
+        <v>105.9</v>
+      </c>
     </row>
-    <row r="227" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:88">
       <c r="A227" t="s">
         <v>39</v>
       </c>
@@ -61972,12 +62653,15 @@
       <c r="CI227" s="1">
         <v>102</v>
       </c>
+      <c r="CJ227" s="1">
+        <v>102</v>
+      </c>
     </row>
-    <row r="228" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:88">
       <c r="CB228" s="1"/>
       <c r="CF228" s="1"/>
     </row>
-    <row r="229" spans="1:87" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:88">
       <c r="CB229" s="1"/>
     </row>
   </sheetData>
@@ -61993,6 +62677,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004D887293C43710468C34A738B97097AF" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1eeb8b92afff55715f8ec3d66b88e394">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e839471c-3f47-4356-a7e7-a250496d6c8c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="08147f69b467f8072fbbadec706f44b3" ns2:_="">
     <xsd:import namespace="e839471c-3f47-4356-a7e7-a250496d6c8c"/>
@@ -62140,15 +62833,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60DDE5EF-B2A7-4243-AC22-9227D8787637}">
   <ds:schemaRefs>
@@ -62166,6 +62850,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91093FD8-BA24-41DB-B21D-7662A96BA764}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0EA44DD-684C-4D97-A3F1-9BDFE6E2089A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -62181,12 +62873,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91093FD8-BA24-41DB-B21D-7662A96BA764}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>